<commit_message>
refactor: remove tone feature and update image handling
- Remove tone-related fields from rooms data structure and UI
- Update Visualizer to use public URLs instead of file streams
- Modify server to serve temp files publicly for API processing
- Update documentation to reflect removal of tone feature
- Change domain references in nginx config
</commit_message>
<xml_diff>
--- a/demo_excel/rooms.xlsx
+++ b/demo_excel/rooms.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\dsqt\tham-vps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\dsqt\tham-vps\demo_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -30,40 +30,19 @@
     <t>style</t>
   </si>
   <si>
-    <t>tone</t>
-  </si>
-  <si>
     <t>Phòng bếp</t>
   </si>
   <si>
     <t>Hiện đại</t>
   </si>
   <si>
-    <t>Trắng</t>
-  </si>
-  <si>
     <t>Scandinavian</t>
   </si>
   <si>
-    <t>Xám</t>
-  </si>
-  <si>
     <t>Cổ điển</t>
   </si>
   <si>
-    <t>Nâu</t>
-  </si>
-  <si>
     <t>Tối giản</t>
-  </si>
-  <si>
-    <t>Xanh</t>
-  </si>
-  <si>
-    <t>Hồng</t>
-  </si>
-  <si>
-    <t>Khác</t>
   </si>
   <si>
     <t>Phòng khách</t>
@@ -467,20 +446,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="88.21875" customWidth="1"/>
+    <col min="4" max="4" width="88.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,524 +469,437 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E31" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E12" r:id="rId11"/>
-    <hyperlink ref="E13" r:id="rId12"/>
-    <hyperlink ref="E14" r:id="rId13"/>
-    <hyperlink ref="E15" r:id="rId14"/>
-    <hyperlink ref="E16" r:id="rId15"/>
-    <hyperlink ref="E17" r:id="rId16"/>
-    <hyperlink ref="E18" r:id="rId17"/>
-    <hyperlink ref="E19" r:id="rId18"/>
-    <hyperlink ref="E20" r:id="rId19"/>
-    <hyperlink ref="E21" r:id="rId20"/>
-    <hyperlink ref="E22" r:id="rId21"/>
-    <hyperlink ref="E23" r:id="rId22"/>
-    <hyperlink ref="E24" r:id="rId23"/>
-    <hyperlink ref="E25" r:id="rId24"/>
-    <hyperlink ref="E26" r:id="rId25"/>
-    <hyperlink ref="E27" r:id="rId26"/>
-    <hyperlink ref="E28" r:id="rId27"/>
-    <hyperlink ref="E29" r:id="rId28"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: remove temporary Excel lock file and update rooms.xlsx
</commit_message>
<xml_diff>
--- a/demo_excel/rooms.xlsx
+++ b/demo_excel/rooms.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Phòng bếp</t>
   </si>
   <si>
-    <t>Hiện đại</t>
-  </si>
-  <si>
-    <t>Scandinavian</t>
-  </si>
-  <si>
     <t>Cổ điển</t>
   </si>
   <si>
@@ -48,9 +42,6 @@
     <t>Phòng khách</t>
   </si>
   <si>
-    <t>Phòng làm việc</t>
-  </si>
-  <si>
     <t>Phòng ngủ</t>
   </si>
   <si>
@@ -73,6 +64,18 @@
   </si>
   <si>
     <t>https://sf-static.upanhlaylink.com/img/image_20251224d1382cf3211cc3a08539cdee0c369535.jpg</t>
+  </si>
+  <si>
+    <t>Phòng sinh hoạt chung</t>
+  </si>
+  <si>
+    <t>Vintage</t>
+  </si>
+  <si>
+    <t>Bắc Âu</t>
+  </si>
+  <si>
+    <t>Bohemian</t>
   </si>
 </sst>
 </file>
@@ -448,13 +451,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
     <col min="4" max="4" width="88.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -469,7 +473,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -483,7 +487,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -494,10 +498,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -508,10 +512,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -522,10 +526,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -536,10 +540,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -550,10 +554,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -564,10 +568,10 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -575,13 +579,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -589,13 +593,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -603,13 +607,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -617,13 +621,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -631,13 +635,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -645,13 +649,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -659,13 +663,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -673,13 +677,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -687,13 +691,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -701,13 +705,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -715,13 +719,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -729,13 +733,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -743,13 +747,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -757,13 +761,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -771,13 +775,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -785,13 +789,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -799,13 +803,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -813,13 +817,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -827,13 +831,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -841,13 +845,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -855,13 +859,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -902,5 +906,6 @@
     <hyperlink ref="D29" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: simplify room filtering and add style filtering for rugs
- Remove style and color filters for rooms, keeping only room type filter
- Add style filtering for rugs to match selected style
- Update CSV formats and upload requirements accordingly
- Refactor options handling to separate room and style updates
</commit_message>
<xml_diff>
--- a/demo_excel/rooms.xlsx
+++ b/demo_excel/rooms.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -27,18 +27,9 @@
     <t>room</t>
   </si>
   <si>
-    <t>style</t>
-  </si>
-  <si>
     <t>Phòng bếp</t>
   </si>
   <si>
-    <t>Cổ điển</t>
-  </si>
-  <si>
-    <t>Tối giản</t>
-  </si>
-  <si>
     <t>Phòng khách</t>
   </si>
   <si>
@@ -67,15 +58,6 @@
   </si>
   <si>
     <t>Phòng sinh hoạt chung</t>
-  </si>
-  <si>
-    <t>Vintage</t>
-  </si>
-  <si>
-    <t>Bắc Âu</t>
-  </si>
-  <si>
-    <t>Bohemian</t>
   </si>
 </sst>
 </file>
@@ -449,20 +431,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
-    <col min="4" max="4" width="88.21875" customWidth="1"/>
+    <col min="3" max="3" width="88.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,440 +451,353 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D31" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C31" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="D10" r:id="rId9"/>
-    <hyperlink ref="D11" r:id="rId10"/>
-    <hyperlink ref="D12" r:id="rId11"/>
-    <hyperlink ref="D13" r:id="rId12"/>
-    <hyperlink ref="D14" r:id="rId13"/>
-    <hyperlink ref="D15" r:id="rId14"/>
-    <hyperlink ref="D16" r:id="rId15"/>
-    <hyperlink ref="D17" r:id="rId16"/>
-    <hyperlink ref="D18" r:id="rId17"/>
-    <hyperlink ref="D19" r:id="rId18"/>
-    <hyperlink ref="D20" r:id="rId19"/>
-    <hyperlink ref="D21" r:id="rId20"/>
-    <hyperlink ref="D22" r:id="rId21"/>
-    <hyperlink ref="D23" r:id="rId22"/>
-    <hyperlink ref="D24" r:id="rId23"/>
-    <hyperlink ref="D25" r:id="rId24"/>
-    <hyperlink ref="D26" r:id="rId25"/>
-    <hyperlink ref="D27" r:id="rId26"/>
-    <hyperlink ref="D28" r:id="rId27"/>
-    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="C17" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C19" r:id="rId18"/>
+    <hyperlink ref="C20" r:id="rId19"/>
+    <hyperlink ref="C21" r:id="rId20"/>
+    <hyperlink ref="C22" r:id="rId21"/>
+    <hyperlink ref="C23" r:id="rId22"/>
+    <hyperlink ref="C24" r:id="rId23"/>
+    <hyperlink ref="C25" r:id="rId24"/>
+    <hyperlink ref="C26" r:id="rId25"/>
+    <hyperlink ref="C27" r:id="rId26"/>
+    <hyperlink ref="C28" r:id="rId27"/>
+    <hyperlink ref="C29" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId29"/>

</xml_diff>

<commit_message>
feat: Introduce a chatbot-guided rug and room selection system with new data, UI, and API endpoints.
</commit_message>
<xml_diff>
--- a/demo_excel/rooms.xlsx
+++ b/demo_excel/rooms.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>Phòng sinh hoạt chung</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>phong-bep</t>
+  </si>
+  <si>
+    <t>phong-khach</t>
+  </si>
+  <si>
+    <t>phong-sinh-hoat-chung</t>
+  </si>
+  <si>
+    <t>phong-ngu</t>
   </si>
 </sst>
 </file>
@@ -431,19 +446,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="88.21875" customWidth="1"/>
+    <col min="2" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="88.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,353 +466,440 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C31" s="2"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
-    <hyperlink ref="C15" r:id="rId14"/>
-    <hyperlink ref="C16" r:id="rId15"/>
-    <hyperlink ref="C17" r:id="rId16"/>
-    <hyperlink ref="C18" r:id="rId17"/>
-    <hyperlink ref="C19" r:id="rId18"/>
-    <hyperlink ref="C20" r:id="rId19"/>
-    <hyperlink ref="C21" r:id="rId20"/>
-    <hyperlink ref="C22" r:id="rId21"/>
-    <hyperlink ref="C23" r:id="rId22"/>
-    <hyperlink ref="C24" r:id="rId23"/>
-    <hyperlink ref="C25" r:id="rId24"/>
-    <hyperlink ref="C26" r:id="rId25"/>
-    <hyperlink ref="C27" r:id="rId26"/>
-    <hyperlink ref="C28" r:id="rId27"/>
-    <hyperlink ref="C29" r:id="rId28"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId29"/>

</xml_diff>